<commit_message>
Add additional analysis based on new thoughts
Signed-off-by: Liang Zhang <psychelzh@outlook.com>
</commit_message>
<xml_diff>
--- a/config/indices_filtering.xlsx
+++ b/config/indices_filtering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e24742936e72e2bc/Documents/Research/cogstruct-dev/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="11_0B09FE74EF773DC4B8A77D7895B3AB5873157DD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F7CB57-7D6B-497D-8FA9-5F05AE7B1DFB}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="11_0B09FE74EF773DC4B8A77D7895B3AB5873157DD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB28DA5-C232-4007-94B1-07D55F5682E5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="592">
   <si>
     <t>game_name_origin</t>
   </si>
@@ -2496,10 +2496,10 @@
   <dimension ref="A1:V403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F93" sqref="F1:F93"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2522,7 @@
     <col min="22" max="22" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0.69652282645294705</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="V3" s="11"/>
     </row>
-    <row r="4" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.73292984007061102</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>0.60906835022055705</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="V6" s="13"/>
     </row>
-    <row r="7" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>0.71346903519898996</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="T12" s="13"/>
       <c r="V12" s="13"/>
     </row>
-    <row r="13" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.26320751415082499</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>0.89836645902107404</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>0.780325195125533</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>586</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="F16" s="12" t="b">
         <v>1</v>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="V16" s="13"/>
     </row>
-    <row r="17" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="V17" s="13"/>
     </row>
-    <row r="18" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>0.92317460562217502</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>0.55381715225474504</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0.85906397227988796</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>0.59951768499814195</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>583</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="F22" s="10" t="b">
         <v>1</v>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="V22" s="11"/>
     </row>
-    <row r="23" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>0.162689435904632</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="V24" s="15"/>
     </row>
-    <row r="25" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>0.75717658511635599</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>0.31436226857518801</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>0.39665155050439899</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>0.954365291012231</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0.92129521321030805</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>0.93062852115942696</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>0.93273980510036403</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>0.95229577136099897</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>0.90939764182508198</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>0.92705958678090095</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>0.94379494032512001</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>0.97936115430290704</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>0.97010335564060701</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>0.95493148537069406</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>0.95988396819815502</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>0.97072514336807803</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>0.93934969900717002</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>0.90632967747472504</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>0.90650172094078996</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>0.88996433636418404</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>0.87254388967672802</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>0.95331410125649396</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0.95524586438032899</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>0.94861182732382199</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>0.95927152740690202</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>0.52610752347952405</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>0.66666849976356402</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>66</v>
       </c>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="V52" s="13"/>
     </row>
-    <row r="53" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>0.15965873952034099</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>-0.438139829125544</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>0.15739405355286401</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>0.88021772383957098</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>0.857531037735347</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>0.71357909856098301</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>0.48216078116630501</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>0.97599462866865705</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0.88377282261606804</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>144</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>144</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="T64" s="13"/>
       <c r="V64" s="13"/>
     </row>
-    <row r="65" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>144</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>0.87389427036987599</v>
       </c>
     </row>
-    <row r="67" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>153</v>
       </c>
@@ -6118,7 +6118,7 @@
       </c>
       <c r="V67" s="13"/>
     </row>
-    <row r="68" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>159</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>0.69293952974444095</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>159</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>0.61912793058188198</v>
       </c>
     </row>
-    <row r="70" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>159</v>
       </c>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="V70" s="13"/>
     </row>
-    <row r="71" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>0.63278241302933702</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>0.51633490988890896</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>0.59334264401220005</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>159</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>0.94359383909933403</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>159</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>0.94095400880955105</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>0.94131104698555201</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>0.94967220259385698</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>0.983082834447914</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>0.94997889028853999</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>0.960270302995195</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>159</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>0.87466744984079503</v>
       </c>
     </row>
-    <row r="82" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>0.86214415911985198</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>159</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>0.79459017880088301</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>159</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>0.94419489063489304</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>0.94905146783293404</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>159</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>0.68802505527124003</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>159</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>0.65832126885040698</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>180</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>0.87368230922387202</v>
       </c>
     </row>
-    <row r="89" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>180</v>
       </c>
@@ -7313,7 +7313,7 @@
       </c>
       <c r="V89" s="13"/>
     </row>
-    <row r="90" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.68458343924146903</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>185</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>0.37340833961974002</v>
       </c>
     </row>
-    <row r="92" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>185</v>
       </c>
@@ -7482,7 +7482,7 @@
       </c>
       <c r="V92" s="13"/>
     </row>
-    <row r="93" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>0.92722323513400595</v>
       </c>
     </row>
-    <row r="94" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>185</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>0.95741857908535899</v>
       </c>
     </row>
-    <row r="95" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>185</v>
       </c>
@@ -7658,7 +7658,7 @@
       </c>
       <c r="V95" s="13"/>
     </row>
-    <row r="96" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>0.85308985320206498</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>185</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>0.90195440937252802</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>185</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>0.86016084993924102</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>-0.112460915148651</v>
       </c>
     </row>
-    <row r="100" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>196</v>
       </c>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="V100" s="13"/>
     </row>
-    <row r="101" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>196</v>
       </c>
@@ -8005,7 +8005,7 @@
       </c>
       <c r="V101" s="13"/>
     </row>
-    <row r="102" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" s="16" t="s">
         <v>202</v>
       </c>
@@ -8050,7 +8050,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
         <v>202</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
         <v>202</v>
       </c>
@@ -8151,7 +8151,7 @@
       <c r="T104" s="13"/>
       <c r="V104" s="13"/>
     </row>
-    <row r="105" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
         <v>202</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>0.82660096084998502</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>208</v>
       </c>
@@ -8311,7 +8311,7 @@
         <v>0.77679785931846002</v>
       </c>
     </row>
-    <row r="108" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>208</v>
       </c>
@@ -8374,7 +8374,7 @@
       </c>
       <c r="V108" s="13"/>
     </row>
-    <row r="109" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>208</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>0.82996967897538898</v>
       </c>
     </row>
-    <row r="110" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>208</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>0.92037114777121898</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>208</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>0.84421158839140198</v>
       </c>
     </row>
-    <row r="112" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>208</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>0.98095637093780097</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>208</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>0.91560621164288902</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>0.94942893035067599</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>208</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>0.96047092710186199</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>208</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>0.97579121604956598</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>208</v>
       </c>
@@ -8851,7 +8851,7 @@
         <v>0.93956132468984299</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>208</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>0.93953545923614401</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>208</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>0.96493713556602001</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>208</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>0.98848866094809495</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>0.98273392009843097</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>208</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>0.97144026280446205</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>208</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>0.97103582750084205</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>208</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>0.97317175904716802</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>208</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>0.88533656800077498</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>0.89111170608280199</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>208</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>0.86109670701809204</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>208</v>
       </c>
@@ -9434,7 +9434,7 @@
         <v>0.77749123077830096</v>
       </c>
     </row>
-    <row r="129" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>208</v>
       </c>
@@ -9487,7 +9487,7 @@
         <v>0.82148480750928898</v>
       </c>
     </row>
-    <row r="130" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>0.98191944178648505</v>
       </c>
     </row>
-    <row r="131" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>208</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>0.93476243393082203</v>
       </c>
     </row>
-    <row r="132" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>208</v>
       </c>
@@ -9646,7 +9646,7 @@
         <v>0.961449165273773</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>0.95972196328191695</v>
       </c>
     </row>
-    <row r="134" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>208</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>0.45446495827086097</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>208</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>0.40969561464123999</v>
       </c>
     </row>
-    <row r="136" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>208</v>
       </c>
@@ -9877,7 +9877,7 @@
       </c>
       <c r="V136" s="13"/>
     </row>
-    <row r="137" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>208</v>
       </c>
@@ -9930,7 +9930,7 @@
         <v>0.18754450726146599</v>
       </c>
     </row>
-    <row r="138" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -9983,7 +9983,7 @@
         <v>0.578816295572399</v>
       </c>
     </row>
-    <row r="139" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>208</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>0.49792372699410797</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>208</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>0.680693703373909</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>208</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>0.69035256251228605</v>
       </c>
     </row>
-    <row r="142" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>208</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>0.626759157374709</v>
       </c>
     </row>
-    <row r="143" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>208</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>0.69140480674907101</v>
       </c>
     </row>
-    <row r="144" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>241</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>241</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>241</v>
       </c>
@@ -10392,7 +10392,7 @@
       <c r="T146" s="13"/>
       <c r="V146" s="13"/>
     </row>
-    <row r="147" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>241</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="18" t="s">
         <v>246</v>
       </c>
@@ -10501,7 +10501,7 @@
       <c r="T148" s="13"/>
       <c r="V148" s="13"/>
     </row>
-    <row r="149" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>249</v>
       </c>
@@ -10557,7 +10557,7 @@
       <c r="T149" s="13"/>
       <c r="V149" s="13"/>
     </row>
-    <row r="150" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>252</v>
       </c>
@@ -10613,7 +10613,7 @@
       <c r="T150" s="13"/>
       <c r="V150" s="13"/>
     </row>
-    <row r="151" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>252</v>
       </c>
@@ -10659,7 +10659,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="152" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>257</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>0.94236685910291296</v>
       </c>
     </row>
-    <row r="153" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>257</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>0.89211739891521202</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>257</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>0.95799255295407404</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>257</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>0.94872111976942797</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>257</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>0.98343034982540201</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>257</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>0.973935169866187</v>
       </c>
     </row>
-    <row r="158" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>257</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>0.96460719127471395</v>
       </c>
     </row>
-    <row r="159" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>257</v>
       </c>
@@ -11083,7 +11083,7 @@
         <v>0.91323034922026103</v>
       </c>
     </row>
-    <row r="160" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>257</v>
       </c>
@@ -11136,7 +11136,7 @@
         <v>0.881235534876736</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>257</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>0.826228904745265</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>257</v>
       </c>
@@ -11242,7 +11242,7 @@
         <v>0.94100747256644701</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>257</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>0.91338054596981599</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>257</v>
       </c>
@@ -11305,6 +11305,15 @@
       <c r="C164" t="s">
         <v>121</v>
       </c>
+      <c r="D164" s="26" t="s">
+        <v>585</v>
+      </c>
+      <c r="E164" s="26" t="s">
+        <v>582</v>
+      </c>
+      <c r="F164" t="b">
+        <v>1</v>
+      </c>
       <c r="G164">
         <v>180</v>
       </c>
@@ -11348,7 +11357,7 @@
         <v>0.61186129557152202</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>257</v>
       </c>
@@ -11401,7 +11410,7 @@
         <v>0.43132986985348498</v>
       </c>
     </row>
-    <row r="166" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>257</v>
       </c>
@@ -11415,7 +11424,7 @@
         <v>125</v>
       </c>
       <c r="E166" s="29" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="F166" s="12" t="b">
         <v>1</v>
@@ -11464,7 +11473,7 @@
       </c>
       <c r="V166" s="13"/>
     </row>
-    <row r="167" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>257</v>
       </c>
@@ -11517,7 +11526,7 @@
         <v>0.50985363994999799</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>257</v>
       </c>
@@ -11570,7 +11579,7 @@
         <v>0.57568242131077296</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>257</v>
       </c>
@@ -11623,7 +11632,7 @@
         <v>0.48495678502609002</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>257</v>
       </c>
@@ -11676,7 +11685,7 @@
         <v>0.73925504401964104</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>257</v>
       </c>
@@ -11729,7 +11738,7 @@
         <v>0.79877613634204103</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>277</v>
       </c>
@@ -11782,7 +11791,7 @@
         <v>0.20814794588664001</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>277</v>
       </c>
@@ -11844,7 +11853,7 @@
         <v>0.96817125406805105</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>277</v>
       </c>
@@ -11897,7 +11906,7 @@
         <v>0.976285854444782</v>
       </c>
     </row>
-    <row r="175" spans="1:22" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>277</v>
       </c>
@@ -11960,7 +11969,7 @@
       </c>
       <c r="V175" s="21"/>
     </row>
-    <row r="176" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>277</v>
       </c>
@@ -12013,7 +12022,7 @@
         <v>0.70677186637288003</v>
       </c>
     </row>
-    <row r="177" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>277</v>
       </c>
@@ -12066,7 +12075,7 @@
         <v>0.96887976423048205</v>
       </c>
     </row>
-    <row r="178" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>277</v>
       </c>
@@ -12119,7 +12128,7 @@
         <v>0.89884337711456397</v>
       </c>
     </row>
-    <row r="179" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>277</v>
       </c>
@@ -12172,7 +12181,7 @@
         <v>0.54099371392484397</v>
       </c>
     </row>
-    <row r="180" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>277</v>
       </c>
@@ -12225,7 +12234,7 @@
         <v>0.60936422693689796</v>
       </c>
     </row>
-    <row r="181" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>287</v>
       </c>
@@ -12281,7 +12290,7 @@
       <c r="T181" s="13"/>
       <c r="V181" s="13"/>
     </row>
-    <row r="182" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>289</v>
       </c>
@@ -12328,7 +12337,7 @@
         <v>0.79692941961948804</v>
       </c>
     </row>
-    <row r="183" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>292</v>
       </c>
@@ -12375,7 +12384,7 @@
         <v>0.60632911937492795</v>
       </c>
     </row>
-    <row r="184" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>289</v>
       </c>
@@ -12422,7 +12431,7 @@
         <v>0.73417065935179104</v>
       </c>
     </row>
-    <row r="185" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>292</v>
       </c>
@@ -12469,7 +12478,7 @@
         <v>0.81044848164250305</v>
       </c>
     </row>
-    <row r="186" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
         <v>289</v>
       </c>
@@ -12528,7 +12537,7 @@
       </c>
       <c r="V186" s="13"/>
     </row>
-    <row r="187" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>292</v>
       </c>
@@ -12575,7 +12584,7 @@
         <v>0.59708971712928705</v>
       </c>
     </row>
-    <row r="188" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>289</v>
       </c>
@@ -12622,7 +12631,7 @@
         <v>0.82445156851694901</v>
       </c>
     </row>
-    <row r="189" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>292</v>
       </c>
@@ -12669,7 +12678,7 @@
         <v>0.844768464223286</v>
       </c>
     </row>
-    <row r="190" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>289</v>
       </c>
@@ -12716,7 +12725,7 @@
         <v>0.84664385471121395</v>
       </c>
     </row>
-    <row r="191" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>292</v>
       </c>
@@ -12763,7 +12772,7 @@
         <v>0.85326813917081401</v>
       </c>
     </row>
-    <row r="192" spans="1:22" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="22" t="s">
         <v>289</v>
       </c>
@@ -12816,7 +12825,7 @@
       </c>
       <c r="V192" s="24"/>
     </row>
-    <row r="193" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>292</v>
       </c>
@@ -12863,7 +12872,7 @@
         <v>0.91029972636981105</v>
       </c>
     </row>
-    <row r="194" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>289</v>
       </c>
@@ -12912,7 +12921,7 @@
         <v>0.681106508009514</v>
       </c>
     </row>
-    <row r="195" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>292</v>
       </c>
@@ -12959,7 +12968,7 @@
         <v>0.74679346219545295</v>
       </c>
     </row>
-    <row r="196" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>289</v>
       </c>
@@ -13006,7 +13015,7 @@
         <v>0.84492587209605896</v>
       </c>
     </row>
-    <row r="197" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>292</v>
       </c>
@@ -13053,7 +13062,7 @@
         <v>0.398299038655267</v>
       </c>
     </row>
-    <row r="198" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>289</v>
       </c>
@@ -13100,7 +13109,7 @@
         <v>0.83709897836832103</v>
       </c>
     </row>
-    <row r="199" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>292</v>
       </c>
@@ -13147,7 +13156,7 @@
         <v>0.84868861222313596</v>
       </c>
     </row>
-    <row r="200" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>289</v>
       </c>
@@ -13194,7 +13203,7 @@
         <v>0.59937796896800499</v>
       </c>
     </row>
-    <row r="201" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>292</v>
       </c>
@@ -13241,7 +13250,7 @@
         <v>0.55162698843761004</v>
       </c>
     </row>
-    <row r="202" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>303</v>
       </c>
@@ -13294,7 +13303,7 @@
         <v>0.56072312604107999</v>
       </c>
     </row>
-    <row r="203" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>303</v>
       </c>
@@ -13357,7 +13366,7 @@
       </c>
       <c r="V203" s="13"/>
     </row>
-    <row r="204" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>303</v>
       </c>
@@ -13417,7 +13426,7 @@
         <v>0.96741883508728799</v>
       </c>
     </row>
-    <row r="205" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>303</v>
       </c>
@@ -13470,7 +13479,7 @@
         <v>0.97555169836845701</v>
       </c>
     </row>
-    <row r="206" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>303</v>
       </c>
@@ -13533,7 +13542,7 @@
       </c>
       <c r="V206" s="13"/>
     </row>
-    <row r="207" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>303</v>
       </c>
@@ -13595,7 +13604,7 @@
         <v>0.88861727031453497</v>
       </c>
     </row>
-    <row r="208" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>303</v>
       </c>
@@ -13648,7 +13657,7 @@
         <v>0.96624817804959895</v>
       </c>
     </row>
-    <row r="209" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>303</v>
       </c>
@@ -13701,7 +13710,7 @@
         <v>0.898768957073522</v>
       </c>
     </row>
-    <row r="210" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>303</v>
       </c>
@@ -13754,7 +13763,7 @@
         <v>0.52605767798331504</v>
       </c>
     </row>
-    <row r="211" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>311</v>
       </c>
@@ -13798,7 +13807,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="212" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>311</v>
       </c>
@@ -13842,7 +13851,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="213" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>311</v>
       </c>
@@ -13898,7 +13907,7 @@
       <c r="T213" s="13"/>
       <c r="V213" s="13"/>
     </row>
-    <row r="214" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>311</v>
       </c>
@@ -13951,7 +13960,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="215" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>316</v>
       </c>
@@ -13995,7 +14004,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="216" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>316</v>
       </c>
@@ -14039,7 +14048,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="217" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>316</v>
       </c>
@@ -14083,7 +14092,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="218" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>316</v>
       </c>
@@ -14127,7 +14136,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="219" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>316</v>
       </c>
@@ -14171,7 +14180,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="220" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>316</v>
       </c>
@@ -14215,7 +14224,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="221" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>316</v>
       </c>
@@ -14259,7 +14268,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="222" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>316</v>
       </c>
@@ -14303,7 +14312,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="223" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>316</v>
       </c>
@@ -14347,7 +14356,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="224" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>326</v>
       </c>
@@ -14400,7 +14409,7 @@
         <v>0.24393656084711299</v>
       </c>
     </row>
-    <row r="225" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>326</v>
       </c>
@@ -14463,7 +14472,7 @@
       </c>
       <c r="V225" s="13"/>
     </row>
-    <row r="226" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>326</v>
       </c>
@@ -14516,7 +14525,7 @@
         <v>0.86130538543086399</v>
       </c>
     </row>
-    <row r="227" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>326</v>
       </c>
@@ -14569,7 +14578,7 @@
         <v>0.88876255709054097</v>
       </c>
     </row>
-    <row r="228" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>326</v>
       </c>
@@ -14632,7 +14641,7 @@
       </c>
       <c r="V228" s="13"/>
     </row>
-    <row r="229" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>326</v>
       </c>
@@ -14685,7 +14694,7 @@
         <v>0.75178686729776101</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>326</v>
       </c>
@@ -14738,7 +14747,7 @@
         <v>0.90646619546038698</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>326</v>
       </c>
@@ -14791,7 +14800,7 @@
         <v>0.78318990861737203</v>
       </c>
     </row>
-    <row r="232" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>326</v>
       </c>
@@ -14844,7 +14853,7 @@
         <v>0.12039005092193</v>
       </c>
     </row>
-    <row r="233" spans="1:22" s="32" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="32" t="s">
         <v>336</v>
       </c>
@@ -14895,7 +14904,7 @@
       <c r="T233" s="34"/>
       <c r="V233" s="34"/>
     </row>
-    <row r="234" spans="1:22" s="37" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="37" t="s">
         <v>336</v>
       </c>
@@ -14946,7 +14955,7 @@
       <c r="T234" s="39"/>
       <c r="V234" s="39"/>
     </row>
-    <row r="235" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>336</v>
       </c>
@@ -14990,7 +14999,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="236" spans="1:22" s="35" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="35" t="s">
         <v>336</v>
       </c>
@@ -15046,7 +15055,7 @@
       <c r="T236" s="36"/>
       <c r="V236" s="36"/>
     </row>
-    <row r="237" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>346</v>
       </c>
@@ -15109,7 +15118,7 @@
       </c>
       <c r="V237" s="13"/>
     </row>
-    <row r="238" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>348</v>
       </c>
@@ -15163,7 +15172,7 @@
         <v>0.74835493540016995</v>
       </c>
     </row>
-    <row r="239" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>350</v>
       </c>
@@ -15204,7 +15213,7 @@
         <v>0.80450978178438703</v>
       </c>
     </row>
-    <row r="240" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>351</v>
       </c>
@@ -15248,7 +15257,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="241" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>351</v>
       </c>
@@ -15292,7 +15301,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="242" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>351</v>
       </c>
@@ -15336,7 +15345,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="243" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>351</v>
       </c>
@@ -15380,7 +15389,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="244" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>351</v>
       </c>
@@ -15424,7 +15433,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="245" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>351</v>
       </c>
@@ -15468,7 +15477,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="246" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>351</v>
       </c>
@@ -15524,7 +15533,7 @@
       <c r="T246" s="13"/>
       <c r="V246" s="13"/>
     </row>
-    <row r="247" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>351</v>
       </c>
@@ -15568,7 +15577,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="248" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>351</v>
       </c>
@@ -15612,7 +15621,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="249" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>351</v>
       </c>
@@ -15656,7 +15665,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="250" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>363</v>
       </c>
@@ -15712,7 +15721,7 @@
       <c r="T250" s="13"/>
       <c r="V250" s="13"/>
     </row>
-    <row r="251" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>363</v>
       </c>
@@ -15756,7 +15765,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="252" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>366</v>
       </c>
@@ -15812,7 +15821,7 @@
       <c r="T252" s="13"/>
       <c r="V252" s="13"/>
     </row>
-    <row r="253" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>366</v>
       </c>
@@ -15856,7 +15865,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="254" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>369</v>
       </c>
@@ -15912,7 +15921,7 @@
       <c r="T254" s="13"/>
       <c r="V254" s="13"/>
     </row>
-    <row r="255" spans="1:22" s="32" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="32" t="s">
         <v>372</v>
       </c>
@@ -15975,7 +15984,7 @@
       </c>
       <c r="V255" s="34"/>
     </row>
-    <row r="256" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>372</v>
       </c>
@@ -16028,7 +16037,7 @@
         <v>0.87446001319920297</v>
       </c>
     </row>
-    <row r="257" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>372</v>
       </c>
@@ -16091,7 +16100,7 @@
       </c>
       <c r="V257" s="13"/>
     </row>
-    <row r="258" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>377</v>
       </c>
@@ -16144,7 +16153,7 @@
         <v>0.439738962581885</v>
       </c>
     </row>
-    <row r="259" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>377</v>
       </c>
@@ -16207,7 +16216,7 @@
       </c>
       <c r="V259" s="13"/>
     </row>
-    <row r="260" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>377</v>
       </c>
@@ -16267,7 +16276,7 @@
         <v>0.96537073088872705</v>
       </c>
     </row>
-    <row r="261" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>377</v>
       </c>
@@ -16320,7 +16329,7 @@
         <v>0.97643771041945604</v>
       </c>
     </row>
-    <row r="262" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>377</v>
       </c>
@@ -16383,7 +16392,7 @@
       </c>
       <c r="V262" s="13"/>
     </row>
-    <row r="263" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>377</v>
       </c>
@@ -16445,7 +16454,7 @@
         <v>0.83538953807416905</v>
       </c>
     </row>
-    <row r="264" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>377</v>
       </c>
@@ -16498,7 +16507,7 @@
         <v>0.97636044769166697</v>
       </c>
     </row>
-    <row r="265" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>377</v>
       </c>
@@ -16551,7 +16560,7 @@
         <v>0.88141700388399402</v>
       </c>
     </row>
-    <row r="266" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>377</v>
       </c>
@@ -16604,7 +16613,7 @@
         <v>0.35507348047276899</v>
       </c>
     </row>
-    <row r="267" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="18" t="s">
         <v>387</v>
       </c>
@@ -16658,7 +16667,7 @@
         <v>0.29209724347296601</v>
       </c>
     </row>
-    <row r="268" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>389</v>
       </c>
@@ -16699,7 +16708,7 @@
         <v>0.25330758628331801</v>
       </c>
     </row>
-    <row r="269" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>390</v>
       </c>
@@ -16743,7 +16752,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="270" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>390</v>
       </c>
@@ -16787,7 +16796,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="271" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>390</v>
       </c>
@@ -16843,7 +16852,7 @@
       <c r="T271" s="13"/>
       <c r="V271" s="13"/>
     </row>
-    <row r="272" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>390</v>
       </c>
@@ -16896,7 +16905,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="273" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>395</v>
       </c>
@@ -16952,7 +16961,7 @@
       <c r="T273" s="13"/>
       <c r="V273" s="13"/>
     </row>
-    <row r="274" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>397</v>
       </c>
@@ -17008,7 +17017,7 @@
       <c r="T274" s="13"/>
       <c r="V274" s="13"/>
     </row>
-    <row r="275" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>399</v>
       </c>
@@ -17070,7 +17079,7 @@
         <v>0.57594975980113905</v>
       </c>
     </row>
-    <row r="276" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>399</v>
       </c>
@@ -17123,7 +17132,7 @@
         <v>0.54372027720553395</v>
       </c>
     </row>
-    <row r="277" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>399</v>
       </c>
@@ -17186,7 +17195,7 @@
       </c>
       <c r="V277" s="13"/>
     </row>
-    <row r="278" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>399</v>
       </c>
@@ -17239,7 +17248,7 @@
         <v>0.50160511397725305</v>
       </c>
     </row>
-    <row r="279" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>399</v>
       </c>
@@ -17292,7 +17301,7 @@
         <v>0.80724618614822696</v>
       </c>
     </row>
-    <row r="280" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>399</v>
       </c>
@@ -17345,7 +17354,7 @@
         <v>0.75349344553745801</v>
       </c>
     </row>
-    <row r="281" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>399</v>
       </c>
@@ -17398,7 +17407,7 @@
         <v>0.97645373263656599</v>
       </c>
     </row>
-    <row r="282" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>399</v>
       </c>
@@ -17451,7 +17460,7 @@
         <v>0.96722403713390004</v>
       </c>
     </row>
-    <row r="283" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>399</v>
       </c>
@@ -17504,7 +17513,7 @@
         <v>0.97288840598926596</v>
       </c>
     </row>
-    <row r="284" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>399</v>
       </c>
@@ -17557,7 +17566,7 @@
         <v>0.97188293398563197</v>
       </c>
     </row>
-    <row r="285" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>399</v>
       </c>
@@ -17610,7 +17619,7 @@
         <v>0.990556891575337</v>
       </c>
     </row>
-    <row r="286" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>399</v>
       </c>
@@ -17663,7 +17672,7 @@
         <v>0.97989155752261803</v>
       </c>
     </row>
-    <row r="287" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>399</v>
       </c>
@@ -17716,7 +17725,7 @@
         <v>0.98233682118185806</v>
       </c>
     </row>
-    <row r="288" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>399</v>
       </c>
@@ -17769,7 +17778,7 @@
         <v>0.797464986295917</v>
       </c>
     </row>
-    <row r="289" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>399</v>
       </c>
@@ -17822,7 +17831,7 @@
         <v>0.55461041397997202</v>
       </c>
     </row>
-    <row r="290" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>399</v>
       </c>
@@ -17875,7 +17884,7 @@
         <v>0.76194823826421199</v>
       </c>
     </row>
-    <row r="291" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>399</v>
       </c>
@@ -17928,7 +17937,7 @@
         <v>0.97960413526393297</v>
       </c>
     </row>
-    <row r="292" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>399</v>
       </c>
@@ -17981,7 +17990,7 @@
         <v>0.97453347233814402</v>
       </c>
     </row>
-    <row r="293" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>399</v>
       </c>
@@ -18034,7 +18043,7 @@
         <v>0.64318405101553999</v>
       </c>
     </row>
-    <row r="294" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>399</v>
       </c>
@@ -18087,7 +18096,7 @@
         <v>0.58986539405056704</v>
       </c>
     </row>
-    <row r="295" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>418</v>
       </c>
@@ -18146,7 +18155,7 @@
       </c>
       <c r="V295" s="13"/>
     </row>
-    <row r="296" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>421</v>
       </c>
@@ -18193,7 +18202,7 @@
         <v>0.84607646378953305</v>
       </c>
     </row>
-    <row r="297" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>418</v>
       </c>
@@ -18240,7 +18249,7 @@
         <v>0.78180324132557399</v>
       </c>
     </row>
-    <row r="298" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>421</v>
       </c>
@@ -18287,7 +18296,7 @@
         <v>0.83232395775935797</v>
       </c>
     </row>
-    <row r="299" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>418</v>
       </c>
@@ -18334,7 +18343,7 @@
         <v>0.83687610275272095</v>
       </c>
     </row>
-    <row r="300" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>421</v>
       </c>
@@ -18381,7 +18390,7 @@
         <v>0.79200033623740995</v>
       </c>
     </row>
-    <row r="301" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>418</v>
       </c>
@@ -18428,7 +18437,7 @@
         <v>0.68591327248409195</v>
       </c>
     </row>
-    <row r="302" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>421</v>
       </c>
@@ -18475,7 +18484,7 @@
         <v>0.64875978292778802</v>
       </c>
     </row>
-    <row r="303" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>418</v>
       </c>
@@ -18522,7 +18531,7 @@
         <v>0.909387897785221</v>
       </c>
     </row>
-    <row r="304" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>421</v>
       </c>
@@ -18569,7 +18578,7 @@
         <v>0.92209057455618704</v>
       </c>
     </row>
-    <row r="305" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>429</v>
       </c>
@@ -18623,7 +18632,7 @@
         <v>0.68345100078370702</v>
       </c>
     </row>
-    <row r="306" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>431</v>
       </c>
@@ -18664,7 +18673,7 @@
         <v>0.82882431704325199</v>
       </c>
     </row>
-    <row r="307" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>432</v>
       </c>
@@ -18718,7 +18727,7 @@
         <v>0.66791515369641896</v>
       </c>
     </row>
-    <row r="308" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>434</v>
       </c>
@@ -18759,7 +18768,7 @@
         <v>0.82344992639495196</v>
       </c>
     </row>
-    <row r="309" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>435</v>
       </c>
@@ -18803,7 +18812,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="310" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>435</v>
       </c>
@@ -18847,7 +18856,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="311" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>435</v>
       </c>
@@ -18903,7 +18912,7 @@
       <c r="T311" s="13"/>
       <c r="V311" s="13"/>
     </row>
-    <row r="312" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>435</v>
       </c>
@@ -18956,7 +18965,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="313" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>440</v>
       </c>
@@ -19009,7 +19018,7 @@
         <v>0.38169174977040998</v>
       </c>
     </row>
-    <row r="314" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>440</v>
       </c>
@@ -19072,7 +19081,7 @@
       </c>
       <c r="V314" s="13"/>
     </row>
-    <row r="315" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>440</v>
       </c>
@@ -19132,7 +19141,7 @@
         <v>0.93201503474775904</v>
       </c>
     </row>
-    <row r="316" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>440</v>
       </c>
@@ -19185,7 +19194,7 @@
         <v>0.95234281359762996</v>
       </c>
     </row>
-    <row r="317" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
         <v>440</v>
       </c>
@@ -19248,7 +19257,7 @@
       </c>
       <c r="V317" s="13"/>
     </row>
-    <row r="318" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>440</v>
       </c>
@@ -19310,7 +19319,7 @@
         <v>0.838977275002181</v>
       </c>
     </row>
-    <row r="319" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>440</v>
       </c>
@@ -19363,7 +19372,7 @@
         <v>0.96779856916885598</v>
       </c>
     </row>
-    <row r="320" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>440</v>
       </c>
@@ -19416,7 +19425,7 @@
         <v>0.865383165440885</v>
       </c>
     </row>
-    <row r="321" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>440</v>
       </c>
@@ -19469,7 +19478,7 @@
         <v>0.166312392592634</v>
       </c>
     </row>
-    <row r="322" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="18" t="s">
         <v>450</v>
       </c>
@@ -19523,7 +19532,7 @@
         <v>0.47727698191569301</v>
       </c>
     </row>
-    <row r="323" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>452</v>
       </c>
@@ -19564,7 +19573,7 @@
         <v>0.60821116606999104</v>
       </c>
     </row>
-    <row r="324" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A324" s="16" t="s">
         <v>453</v>
       </c>
@@ -19609,7 +19618,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="325" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A325" s="16" t="s">
         <v>453</v>
       </c>
@@ -19654,7 +19663,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="326" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A326" s="18" t="s">
         <v>453</v>
       </c>
@@ -19710,7 +19719,7 @@
       <c r="T326" s="13"/>
       <c r="V326" s="13"/>
     </row>
-    <row r="327" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A327" s="16" t="s">
         <v>453</v>
       </c>
@@ -19755,7 +19764,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="328" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A328" s="18" t="s">
         <v>463</v>
       </c>
@@ -19811,7 +19820,7 @@
       <c r="T328" s="13"/>
       <c r="V328" s="13"/>
     </row>
-    <row r="329" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="18" t="s">
         <v>463</v>
       </c>
@@ -19867,7 +19876,7 @@
       <c r="T329" s="13"/>
       <c r="V329" s="13"/>
     </row>
-    <row r="330" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>467</v>
       </c>
@@ -19911,7 +19920,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="331" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>467</v>
       </c>
@@ -19955,7 +19964,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="332" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
         <v>467</v>
       </c>
@@ -20011,7 +20020,7 @@
       <c r="T332" s="13"/>
       <c r="V332" s="13"/>
     </row>
-    <row r="333" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>467</v>
       </c>
@@ -20064,7 +20073,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="334" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="s">
         <v>472</v>
       </c>
@@ -20120,7 +20129,7 @@
       <c r="T334" s="13"/>
       <c r="V334" s="13"/>
     </row>
-    <row r="335" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>474</v>
       </c>
@@ -20176,7 +20185,7 @@
         <v>0.742345301146632</v>
       </c>
     </row>
-    <row r="336" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>477</v>
       </c>
@@ -20223,7 +20232,7 @@
         <v>0.83402932112545003</v>
       </c>
     </row>
-    <row r="337" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
         <v>474</v>
       </c>
@@ -20282,7 +20291,7 @@
       </c>
       <c r="V337" s="13"/>
     </row>
-    <row r="338" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>477</v>
       </c>
@@ -20329,7 +20338,7 @@
         <v>3.4988954723256402E-2</v>
       </c>
     </row>
-    <row r="339" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>474</v>
       </c>
@@ -20376,7 +20385,7 @@
         <v>0.54359528712977001</v>
       </c>
     </row>
-    <row r="340" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>477</v>
       </c>
@@ -20423,7 +20432,7 @@
         <v>0.63293804372958595</v>
       </c>
     </row>
-    <row r="341" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
         <v>474</v>
       </c>
@@ -20482,7 +20491,7 @@
       </c>
       <c r="V341" s="13"/>
     </row>
-    <row r="342" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>477</v>
       </c>
@@ -20529,7 +20538,7 @@
         <v>0.84903275513532905</v>
       </c>
     </row>
-    <row r="343" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>484</v>
       </c>
@@ -20582,7 +20591,7 @@
         <v>0.88586030500857205</v>
       </c>
     </row>
-    <row r="344" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
         <v>484</v>
       </c>
@@ -20645,7 +20654,7 @@
       </c>
       <c r="V344" s="13"/>
     </row>
-    <row r="345" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>484</v>
       </c>
@@ -20698,7 +20707,7 @@
         <v>0.84377155015479299</v>
       </c>
     </row>
-    <row r="346" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>484</v>
       </c>
@@ -20751,7 +20760,7 @@
         <v>0.86224759631480496</v>
       </c>
     </row>
-    <row r="347" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>484</v>
       </c>
@@ -20804,7 +20813,7 @@
         <v>0.89826776073858094</v>
       </c>
     </row>
-    <row r="348" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>484</v>
       </c>
@@ -20857,7 +20866,7 @@
         <v>0.794125510388904</v>
       </c>
     </row>
-    <row r="349" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>484</v>
       </c>
@@ -20910,7 +20919,7 @@
         <v>0.86419130634230401</v>
       </c>
     </row>
-    <row r="350" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>484</v>
       </c>
@@ -20963,7 +20972,7 @@
         <v>0.90110654307701499</v>
       </c>
     </row>
-    <row r="351" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>484</v>
       </c>
@@ -21016,7 +21025,7 @@
         <v>0.82433547664307005</v>
       </c>
     </row>
-    <row r="352" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>484</v>
       </c>
@@ -21069,7 +21078,7 @@
         <v>0.87081873951669497</v>
       </c>
     </row>
-    <row r="353" spans="1:22" s="32" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="32" t="s">
         <v>484</v>
       </c>
@@ -21132,7 +21141,7 @@
       </c>
       <c r="V353" s="34"/>
     </row>
-    <row r="354" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>484</v>
       </c>
@@ -21185,7 +21194,7 @@
         <v>0.835936410919495</v>
       </c>
     </row>
-    <row r="355" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>484</v>
       </c>
@@ -21238,7 +21247,7 @@
         <v>0.89201603007758801</v>
       </c>
     </row>
-    <row r="356" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>484</v>
       </c>
@@ -21291,7 +21300,7 @@
         <v>0.92894372923318702</v>
       </c>
     </row>
-    <row r="357" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>484</v>
       </c>
@@ -21344,7 +21353,7 @@
         <v>0.82916743990848596</v>
       </c>
     </row>
-    <row r="358" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>484</v>
       </c>
@@ -21397,7 +21406,7 @@
         <v>0.93330563256614496</v>
       </c>
     </row>
-    <row r="359" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>484</v>
       </c>
@@ -21450,7 +21459,7 @@
         <v>0.95616336250419898</v>
       </c>
     </row>
-    <row r="360" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>484</v>
       </c>
@@ -21503,7 +21512,7 @@
         <v>0.91633874468938503</v>
       </c>
     </row>
-    <row r="361" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>518</v>
       </c>
@@ -21547,7 +21556,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="362" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>518</v>
       </c>
@@ -21591,7 +21600,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="363" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>518</v>
       </c>
@@ -21635,7 +21644,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="364" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>518</v>
       </c>
@@ -21679,7 +21688,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="365" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>518</v>
       </c>
@@ -21723,7 +21732,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="366" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>518</v>
       </c>
@@ -21767,7 +21776,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="367" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="s">
         <v>518</v>
       </c>
@@ -21823,7 +21832,7 @@
       <c r="T367" s="13"/>
       <c r="V367" s="13"/>
     </row>
-    <row r="368" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>518</v>
       </c>
@@ -21867,7 +21876,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="369" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>518</v>
       </c>
@@ -21911,7 +21920,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="370" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>518</v>
       </c>
@@ -21955,7 +21964,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="371" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>529</v>
       </c>
@@ -21999,7 +22008,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="372" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>529</v>
       </c>
@@ -22043,7 +22052,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="373" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3" t="s">
         <v>529</v>
       </c>
@@ -22099,7 +22108,7 @@
       <c r="T373" s="13"/>
       <c r="V373" s="13"/>
     </row>
-    <row r="374" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>529</v>
       </c>
@@ -22143,7 +22152,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="375" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>534</v>
       </c>
@@ -22187,7 +22196,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="376" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>534</v>
       </c>
@@ -22231,7 +22240,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="377" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
         <v>534</v>
       </c>
@@ -22287,7 +22296,7 @@
       <c r="T377" s="13"/>
       <c r="V377" s="13"/>
     </row>
-    <row r="378" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>534</v>
       </c>
@@ -22340,7 +22349,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="379" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>539</v>
       </c>
@@ -22384,7 +22393,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="380" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>539</v>
       </c>
@@ -22428,7 +22437,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="381" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>539</v>
       </c>
@@ -22472,7 +22481,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="382" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>539</v>
       </c>
@@ -22516,7 +22525,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="383" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>539</v>
       </c>
@@ -22560,7 +22569,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="384" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>539</v>
       </c>
@@ -22604,7 +22613,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="385" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="3" t="s">
         <v>539</v>
       </c>
@@ -22660,7 +22669,7 @@
       <c r="T385" s="13"/>
       <c r="V385" s="13"/>
     </row>
-    <row r="386" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>539</v>
       </c>
@@ -22704,7 +22713,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="387" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>539</v>
       </c>
@@ -22748,7 +22757,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="388" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>539</v>
       </c>
@@ -22792,7 +22801,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="389" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
         <v>550</v>
       </c>
@@ -22846,7 +22855,7 @@
         <v>0.86205785121791201</v>
       </c>
     </row>
-    <row r="390" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>552</v>
       </c>
@@ -22887,7 +22896,7 @@
         <v>0.79938682451651499</v>
       </c>
     </row>
-    <row r="391" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="3" t="s">
         <v>553</v>
       </c>
@@ -22943,7 +22952,7 @@
       <c r="T391" s="13"/>
       <c r="V391" s="13"/>
     </row>
-    <row r="392" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>555</v>
       </c>
@@ -22996,7 +23005,7 @@
         <v>0.43382527625184802</v>
       </c>
     </row>
-    <row r="393" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>555</v>
       </c>
@@ -23049,7 +23058,7 @@
         <v>0.85743481772590602</v>
       </c>
     </row>
-    <row r="394" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="3" t="s">
         <v>555</v>
       </c>
@@ -23112,7 +23121,7 @@
       </c>
       <c r="V394" s="13"/>
     </row>
-    <row r="395" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>555</v>
       </c>
@@ -23165,7 +23174,7 @@
         <v>0.97049595234328201</v>
       </c>
     </row>
-    <row r="396" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>555</v>
       </c>
@@ -23218,7 +23227,7 @@
         <v>0.96195187902225099</v>
       </c>
     </row>
-    <row r="397" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="s">
         <v>555</v>
       </c>
@@ -23281,7 +23290,7 @@
       </c>
       <c r="V397" s="13"/>
     </row>
-    <row r="398" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>555</v>
       </c>
@@ -23334,7 +23343,7 @@
         <v>0.87635220153964399</v>
       </c>
     </row>
-    <row r="399" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>555</v>
       </c>
@@ -23387,7 +23396,7 @@
         <v>0.730811382579868</v>
       </c>
     </row>
-    <row r="400" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>555</v>
       </c>
@@ -23440,7 +23449,7 @@
         <v>0.97049804266529904</v>
       </c>
     </row>
-    <row r="401" spans="1:22" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A401" s="3" t="s">
         <v>555</v>
       </c>
@@ -23503,7 +23512,7 @@
       </c>
       <c r="V401" s="13"/>
     </row>
-    <row r="402" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>565</v>
       </c>
@@ -23520,7 +23529,7 @@
         <v>0.73648325021324601</v>
       </c>
     </row>
-    <row r="403" spans="1:22" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>565</v>
       </c>
@@ -23549,6 +23558,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+</pixelators>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <commentList sheetStid="1">
     <comment s:ref="B22" rgbClr="FF0000">
@@ -23573,13 +23589,6 @@
 </comments>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-</pixelators>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
@@ -23594,6 +23603,12 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A0048C-2381-489B-AA07-9611017176EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
@@ -23602,12 +23617,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
   <ds:schemaRefs/>

</xml_diff>

<commit_message>
Remove strategic rt indices
Signed-off-by: Liang Zhang <psychelzh@outlook.com>
</commit_message>
<xml_diff>
--- a/config/indices_filtering.xlsx
+++ b/config/indices_filtering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e24742936e72e2bc/Documents/Research/cogstruct-dev/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="11_0B09FE74EF773DC4B8A77D7895B3AB5873157DD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB28DA5-C232-4007-94B1-07D55F5682E5}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="11_0B09FE74EF773DC4B8A77D7895B3AB5873157DD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27EF9156-1E0E-4FFD-A795-AE7E7F10977F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="593">
   <si>
     <t>game_name_origin</t>
   </si>
@@ -1881,6 +1881,9 @@
   <si>
     <t>working memory</t>
     <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>target-stash</t>
   </si>
 </sst>
 </file>
@@ -2496,10 +2499,10 @@
   <dimension ref="A1:V403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D221" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -5718,6 +5721,15 @@
       <c r="C60" t="s">
         <v>54</v>
       </c>
+      <c r="D60" s="26" t="s">
+        <v>586</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>582</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
       <c r="G60">
         <v>196</v>
       </c>
@@ -7609,7 +7621,7 @@
         <v>587</v>
       </c>
       <c r="E95" s="29" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F95" s="12" t="b">
         <v>1</v>
@@ -13493,7 +13505,7 @@
         <v>587</v>
       </c>
       <c r="E206" s="29" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F206" s="12" t="b">
         <v>1</v>
@@ -14592,7 +14604,7 @@
         <v>587</v>
       </c>
       <c r="E228" s="29" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="F228" s="12" t="b">
         <v>1</v>
@@ -15935,7 +15947,7 @@
         <v>586</v>
       </c>
       <c r="E255" s="33" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F255" s="33" t="b">
         <v>1</v>
@@ -16343,7 +16355,7 @@
         <v>587</v>
       </c>
       <c r="E262" s="29" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F262" s="12" t="b">
         <v>1</v>
@@ -19208,7 +19220,7 @@
         <v>587</v>
       </c>
       <c r="E317" s="29" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F317" s="12" t="b">
         <v>1</v>
@@ -21092,7 +21104,7 @@
         <v>587</v>
       </c>
       <c r="E353" s="33" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="F353" s="33" t="b">
         <v>1</v>
@@ -23558,13 +23570,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-</pixelators>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <commentList sheetStid="1">
     <comment s:ref="B22" rgbClr="FF0000">
@@ -23589,6 +23594,13 @@
 </comments>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+</pixelators>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
@@ -23603,12 +23615,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A0048C-2381-489B-AA07-9611017176EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
@@ -23617,6 +23623,12 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
   <ds:schemaRefs/>

</xml_diff>